<commit_message>
neuer PAtient Registrierung OK
</commit_message>
<xml_diff>
--- a/Database/Patienten_Zahnärzte_Kosten.xlsx
+++ b/Database/Patienten_Zahnärzte_Kosten.xlsx
@@ -1672,9 +1672,21 @@
       <c r="K29" s="2" t="n"/>
     </row>
     <row r="30" ht="15" customHeight="1">
-      <c r="C30" s="2" t="n"/>
-      <c r="D30" s="2" t="n"/>
-      <c r="E30" s="2" t="n"/>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>freiwillig gesetzlich</t>
+        </is>
+      </c>
       <c r="F30" s="2" t="n"/>
       <c r="G30" s="2" t="n"/>
       <c r="H30" s="2" t="n"/>
@@ -1683,9 +1695,21 @@
       <c r="K30" s="2" t="n"/>
     </row>
     <row r="31" ht="15" customHeight="1">
-      <c r="C31" s="31" t="n"/>
-      <c r="D31" s="31" t="n"/>
-      <c r="E31" s="31" t="n"/>
+      <c r="C31" s="31" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D31" s="31" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E31" s="31" t="inlineStr">
+        <is>
+          <t>freiwillig gesetzlich</t>
+        </is>
+      </c>
       <c r="F31" s="31" t="n"/>
       <c r="G31" s="31" t="n"/>
       <c r="H31" s="31" t="n"/>
@@ -1694,39 +1718,136 @@
       <c r="K31" s="31" t="n"/>
     </row>
     <row r="32" ht="15" customHeight="1">
-      <c r="C32" s="31" t="n"/>
-      <c r="D32" s="31" t="n"/>
-      <c r="E32" s="31" t="n"/>
-      <c r="F32" s="31" t="n"/>
-      <c r="G32" s="31" t="n"/>
+      <c r="C32" s="31" t="inlineStr">
+        <is>
+          <t>Ericka</t>
+        </is>
+      </c>
+      <c r="D32" s="31" t="inlineStr">
+        <is>
+          <t>kala</t>
+        </is>
+      </c>
+      <c r="E32" s="31" t="inlineStr">
+        <is>
+          <t>gesetzlich</t>
+        </is>
+      </c>
+      <c r="F32" s="31" t="inlineStr">
+        <is>
+          <t>Karies groß</t>
+        </is>
+      </c>
+      <c r="G32" s="31" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="H32" s="31" t="n"/>
       <c r="I32" s="31" t="n"/>
       <c r="J32" s="31" t="n"/>
       <c r="K32" s="31" t="n"/>
     </row>
     <row r="33" ht="15" customHeight="1">
-      <c r="G33" s="31" t="n"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>erika</t>
+        </is>
+      </c>
+      <c r="G33" s="31" t="inlineStr"/>
       <c r="H33" s="31" t="n"/>
       <c r="I33" s="31" t="n"/>
       <c r="J33" s="31" t="n"/>
       <c r="K33" s="31" t="n"/>
     </row>
     <row r="34" ht="15" customHeight="1">
-      <c r="G34" s="31" t="n"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Theodore</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>kala</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>gesetzlich</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Teilkrone, Teilkrone</t>
+        </is>
+      </c>
+      <c r="G34" s="31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="H34" s="31" t="n"/>
       <c r="I34" s="31" t="n"/>
       <c r="J34" s="31" t="n"/>
       <c r="K34" s="31" t="n"/>
     </row>
     <row r="35" ht="15" customHeight="1">
-      <c r="G35" s="31" t="n"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Theodore2</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>kala</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>gesetzlich</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Teilkrone</t>
+        </is>
+      </c>
+      <c r="G35" s="31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="H35" s="31" t="n"/>
       <c r="I35" s="31" t="n"/>
       <c r="J35" s="31" t="n"/>
       <c r="K35" s="31" t="n"/>
     </row>
     <row r="36" ht="42" customHeight="1">
-      <c r="G36" s="31" t="n"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Theodore benji</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>kala</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>gesetzlich</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Teilkrone</t>
+        </is>
+      </c>
+      <c r="G36" s="31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="H36" s="31" t="n"/>
     </row>
     <row r="37" ht="15" customHeight="1">
@@ -2863,7 +2984,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" activeCellId="0" sqref="B2:E2"/>
@@ -3020,6 +3141,23 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>theodore</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>theodore</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>freiwillig gesetzlich</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>